<commit_message>
Add landuse mask and fix error with timing of applying r_mask
</commit_message>
<xml_diff>
--- a/ExcelInputs/Rotation.xlsx
+++ b/ExcelInputs/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="117">
   <si>
     <t>AAAA2A1a</t>
   </si>
@@ -121,133 +121,130 @@
     <t>YYWFWb</t>
   </si>
   <si>
+    <t>YYLWNw</t>
+  </si>
+  <si>
+    <t>YYWLWz</t>
+  </si>
+  <si>
+    <t>YYNWLw</t>
+  </si>
+  <si>
+    <t>AYAA2A1w</t>
+  </si>
+  <si>
+    <t>AAWA2A1a</t>
+  </si>
+  <si>
+    <t>AAAWA1a</t>
+  </si>
+  <si>
+    <t>YAAA2Wa</t>
+  </si>
+  <si>
+    <t>YAAA2Nw</t>
+  </si>
+  <si>
+    <t>YYAA2A1z</t>
+  </si>
+  <si>
+    <t>AYWA2A1a</t>
+  </si>
+  <si>
+    <t>AANWA1a</t>
+  </si>
+  <si>
+    <t>AAANWa</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>SP</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>Ag2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>Ag1</t>
+  </si>
+  <si>
+    <t>Sg1</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>OF</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>sp</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bd</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
     <t>YYWNWl</t>
-  </si>
-  <si>
-    <t>YYLWNw</t>
-  </si>
-  <si>
-    <t>YYWLWz</t>
-  </si>
-  <si>
-    <t>YYNWLw</t>
-  </si>
-  <si>
-    <t>AYAA2A1w</t>
-  </si>
-  <si>
-    <t>AAWA2A1a</t>
-  </si>
-  <si>
-    <t>AAAWA1a</t>
-  </si>
-  <si>
-    <t>YAAA2Wa</t>
-  </si>
-  <si>
-    <t>YAAA2Nw</t>
-  </si>
-  <si>
-    <t>YYAA2A1z</t>
-  </si>
-  <si>
-    <t>AYWA2A1a</t>
-  </si>
-  <si>
-    <t>AANWA1a</t>
-  </si>
-  <si>
-    <t>AAANWa</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>SP</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>Ag2</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>Ag1</t>
-  </si>
-  <si>
-    <t>Sg1</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>OF</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>sp</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>bd</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>l</t>
   </si>
   <si>
     <t>AAAA2A1</t>
@@ -728,7 +725,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -739,22 +736,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -762,22 +759,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -785,22 +782,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -808,22 +805,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -831,22 +828,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -854,22 +851,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -877,22 +874,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -900,22 +897,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -923,22 +920,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -946,22 +943,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -969,22 +966,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -992,22 +989,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="C12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
-      </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1015,22 +1012,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1038,22 +1035,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
         <v>50</v>
       </c>
-      <c r="D14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" t="s">
-        <v>51</v>
-      </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1061,22 +1058,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1084,22 +1081,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1107,22 +1104,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1130,22 +1127,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" t="s">
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" t="s">
-        <v>51</v>
-      </c>
       <c r="G18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1153,22 +1150,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" t="s">
         <v>50</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" t="s">
         <v>50</v>
       </c>
-      <c r="D19" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" t="s">
-        <v>51</v>
-      </c>
       <c r="G19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1176,22 +1173,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" t="s">
         <v>50</v>
       </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" t="s">
-        <v>51</v>
-      </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1199,22 +1196,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
         <v>50</v>
       </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
       <c r="F21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1222,22 +1219,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" t="s">
         <v>50</v>
       </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" t="s">
-        <v>51</v>
-      </c>
       <c r="E22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F22" t="s">
         <v>53</v>
       </c>
-      <c r="F22" t="s">
-        <v>54</v>
-      </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1245,22 +1242,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1268,22 +1265,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1291,22 +1288,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
         <v>53</v>
       </c>
-      <c r="F25" t="s">
-        <v>54</v>
-      </c>
       <c r="G25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1314,22 +1311,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" t="s">
         <v>53</v>
       </c>
-      <c r="E26" t="s">
-        <v>54</v>
-      </c>
       <c r="F26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1337,22 +1334,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" t="s">
+        <v>53</v>
+      </c>
+      <c r="E27" t="s">
         <v>50</v>
       </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" t="s">
-        <v>51</v>
-      </c>
       <c r="F27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1360,22 +1357,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" t="s">
         <v>50</v>
       </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" t="s">
-        <v>51</v>
-      </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1383,22 +1380,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1406,22 +1403,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1429,22 +1426,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" t="s">
         <v>50</v>
       </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>55</v>
-      </c>
-      <c r="E31" t="s">
-        <v>54</v>
-      </c>
-      <c r="F31" t="s">
-        <v>51</v>
-      </c>
       <c r="G31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1452,22 +1449,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
         <v>50</v>
       </c>
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" t="s">
-        <v>51</v>
-      </c>
       <c r="E32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" t="s">
         <v>53</v>
       </c>
-      <c r="F32" t="s">
-        <v>54</v>
-      </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1475,22 +1472,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33" t="s">
         <v>53</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>54</v>
       </c>
-      <c r="F33" t="s">
-        <v>55</v>
-      </c>
       <c r="G33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1498,22 +1495,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E34" t="s">
         <v>54</v>
       </c>
-      <c r="E34" t="s">
-        <v>55</v>
-      </c>
       <c r="F34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1521,22 +1518,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E35" t="s">
         <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G35" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1544,22 +1541,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F36" t="s">
         <v>53</v>
       </c>
       <c r="G36" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1567,22 +1564,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F37" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1590,22 +1587,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E38" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F38" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1613,22 +1610,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E39" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G39" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1636,22 +1633,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E40" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1659,22 +1656,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F41" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="G41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1682,22 +1679,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E42" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G42" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1705,22 +1702,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E43" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F43" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G43" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1728,22 +1725,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D44" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G44" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1751,22 +1748,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E45" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1774,45 +1771,22 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" t="s">
         <v>53</v>
       </c>
-      <c r="E46" t="s">
-        <v>54</v>
-      </c>
-      <c r="F46" t="s">
-        <v>60</v>
-      </c>
       <c r="G46" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>47</v>
-      </c>
-      <c r="C47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" t="s">
-        <v>53</v>
-      </c>
-      <c r="F47" t="s">
-        <v>54</v>
-      </c>
-      <c r="G47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1833,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1844,7 +1818,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1855,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1866,7 +1840,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1877,7 +1851,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1888,7 +1862,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1899,7 +1873,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1910,7 +1884,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1921,7 +1895,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1932,7 +1906,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1943,7 +1917,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1954,7 +1928,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1965,7 +1939,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1976,7 +1950,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1987,7 +1961,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1998,7 +1972,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2009,7 +1983,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2020,7 +1994,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2031,7 +2005,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2042,7 +2016,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2053,7 +2027,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2064,7 +2038,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2075,7 +2049,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2086,7 +2060,7 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2097,7 +2071,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2108,7 +2082,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2119,7 +2093,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2130,7 +2104,7 @@
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2141,7 +2115,7 @@
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2152,7 +2126,7 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2163,7 +2137,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2174,7 +2148,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2185,7 +2159,7 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2196,7 +2170,7 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2207,7 +2181,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2218,7 +2192,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2229,7 +2203,7 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2240,7 +2214,7 @@
         <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2251,7 +2225,7 @@
         <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2262,7 +2236,7 @@
         <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2273,7 +2247,7 @@
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2284,7 +2258,7 @@
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2295,7 +2269,7 @@
         <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2306,7 +2280,7 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2317,7 +2291,7 @@
         <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2328,7 +2302,7 @@
         <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2339,7 +2313,7 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -2350,7 +2324,7 @@
         <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2361,7 +2335,7 @@
         <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2372,7 +2346,7 @@
         <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2383,7 +2357,7 @@
         <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2394,7 +2368,7 @@
         <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2405,7 +2379,7 @@
         <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2416,7 +2390,7 @@
         <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2427,7 +2401,7 @@
         <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2438,7 +2412,7 @@
         <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2449,7 +2423,7 @@
         <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2460,7 +2434,7 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2471,7 +2445,7 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2482,7 +2456,7 @@
         <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2493,7 +2467,7 @@
         <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2501,10 +2475,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2512,10 +2486,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -2523,10 +2497,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B64" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -2534,10 +2508,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2545,10 +2519,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2556,10 +2530,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -2567,10 +2541,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -2578,10 +2552,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2589,10 +2563,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -2600,10 +2574,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2611,10 +2585,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B72" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2622,10 +2596,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2633,10 +2607,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B74" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2644,10 +2618,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -2655,10 +2629,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -2666,10 +2640,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B77" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2677,10 +2651,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2688,10 +2662,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -2699,10 +2673,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2710,10 +2684,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -2721,10 +2695,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2732,10 +2706,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B83" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2743,10 +2717,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -2754,10 +2728,10 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -2765,10 +2739,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B86" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -2776,10 +2750,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -2803,7 +2777,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -2814,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -2825,7 +2799,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -2836,7 +2810,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -2847,7 +2821,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -2858,7 +2832,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -2869,7 +2843,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -2880,7 +2854,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -2891,7 +2865,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -2902,7 +2876,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -2913,7 +2887,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2924,7 +2898,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -2935,7 +2909,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -2946,7 +2920,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -2957,7 +2931,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2968,7 +2942,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -2979,7 +2953,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -2990,7 +2964,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -3001,7 +2975,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -3012,7 +2986,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -3023,7 +2997,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -3034,7 +3008,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -3045,7 +3019,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -3056,7 +3030,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -3067,7 +3041,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -3078,7 +3052,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -3089,7 +3063,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -3100,7 +3074,7 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -3111,7 +3085,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -3122,7 +3096,7 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -3133,7 +3107,7 @@
         <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -3144,7 +3118,7 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -3155,7 +3129,7 @@
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -3166,7 +3140,7 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -3177,7 +3151,7 @@
         <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -3188,7 +3162,7 @@
         <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -3199,7 +3173,7 @@
         <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -3210,7 +3184,7 @@
         <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -3221,7 +3195,7 @@
         <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -3232,7 +3206,7 @@
         <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C40">
         <v>-1</v>
@@ -3243,7 +3217,7 @@
         <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C41">
         <v>-1</v>
@@ -3254,7 +3228,7 @@
         <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C42">
         <v>-1</v>
@@ -3265,7 +3239,7 @@
         <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C43">
         <v>-1</v>
@@ -3276,7 +3250,7 @@
         <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44">
         <v>-1</v>
@@ -3287,7 +3261,7 @@
         <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C45">
         <v>-1</v>
@@ -3298,7 +3272,7 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C46">
         <v>-1</v>
@@ -3309,7 +3283,7 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47">
         <v>-1</v>
@@ -3320,7 +3294,7 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C48">
         <v>-1</v>
@@ -3331,7 +3305,7 @@
         <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C49">
         <v>-1</v>
@@ -3342,7 +3316,7 @@
         <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C50">
         <v>-1</v>
@@ -3350,10 +3324,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C51">
         <v>-1</v>
@@ -3361,10 +3335,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C52">
         <v>-1</v>
@@ -3372,10 +3346,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C53">
         <v>-1</v>
@@ -3383,10 +3357,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C54">
         <v>-1</v>
@@ -3394,10 +3368,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55">
         <v>-1</v>
@@ -3405,10 +3379,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C56">
         <v>-1</v>
@@ -3416,10 +3390,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57">
         <v>-1</v>
@@ -3427,10 +3401,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -3438,10 +3412,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C59">
         <v>-1</v>
@@ -3449,10 +3423,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B60" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C60">
         <v>-1</v>
@@ -3460,10 +3434,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B61" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C61">
         <v>-1</v>
@@ -3471,10 +3445,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62">
         <v>-1</v>
@@ -3482,10 +3456,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C63">
         <v>-1</v>
@@ -3493,10 +3467,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B64" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64">
         <v>-1</v>
@@ -3504,10 +3478,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C65">
         <v>-1</v>
@@ -3515,10 +3489,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B66" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C66">
         <v>-1</v>
@@ -3526,10 +3500,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C67">
         <v>-1</v>
@@ -3537,10 +3511,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68">
         <v>-1</v>
@@ -3548,10 +3522,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C69">
         <v>-1</v>
@@ -3559,10 +3533,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C70">
         <v>-1</v>
@@ -3570,10 +3544,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C71">
         <v>-1</v>
@@ -3581,10 +3555,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C72">
         <v>-1</v>
@@ -3592,10 +3566,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C73">
         <v>-1</v>
@@ -3603,10 +3577,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C74">
         <v>-1</v>
@@ -3614,10 +3588,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C75">
         <v>-1</v>
@@ -3625,10 +3599,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C76">
         <v>-1</v>
@@ -3649,822 +3623,822 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" t="s">
         <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
         <v>50</v>
       </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" t="s">
-        <v>51</v>
-      </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>51</v>
-      </c>
       <c r="F12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
         <v>50</v>
       </c>
-      <c r="C26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" t="s">
-        <v>51</v>
-      </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B29" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" t="s">
         <v>50</v>
       </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" t="s">
-        <v>51</v>
-      </c>
       <c r="E29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
         <v>50</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
+        <v>52</v>
+      </c>
+      <c r="F30" t="s">
         <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" t="s">
         <v>50</v>
       </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>51</v>
-      </c>
       <c r="E31" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" t="s">
         <v>53</v>
-      </c>
-      <c r="F31" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s">
         <v>50</v>
-      </c>
-      <c r="C32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F32" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" t="s">
         <v>50</v>
       </c>
-      <c r="C34" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" t="s">
-        <v>51</v>
-      </c>
       <c r="F34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
         <v>50</v>
-      </c>
-      <c r="C35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" t="s">
-        <v>54</v>
-      </c>
-      <c r="F35" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" t="s">
         <v>53</v>
       </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
         <v>54</v>
-      </c>
-      <c r="F36" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" t="s">
         <v>53</v>
       </c>
-      <c r="E37" t="s">
-        <v>54</v>
-      </c>
       <c r="F37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="s">
         <v>50</v>
       </c>
-      <c r="C38" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" t="s">
-        <v>51</v>
-      </c>
       <c r="F38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D39" t="s">
+        <v>53</v>
+      </c>
+      <c r="E39" t="s">
         <v>54</v>
       </c>
-      <c r="E39" t="s">
-        <v>55</v>
-      </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" t="s">
         <v>53</v>
-      </c>
-      <c r="F41" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweaks to make rotation handling better and stop web app error - no profit change
</commit_message>
<xml_diff>
--- a/ExcelInputs/Rotation.xlsx
+++ b/ExcelInputs/Rotation.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="118">
   <si>
     <t>AAAA2A1a</t>
   </si>
@@ -121,6 +121,9 @@
     <t>YYWFWb</t>
   </si>
   <si>
+    <t>YYWNWl</t>
+  </si>
+  <si>
     <t>YYLWNw</t>
   </si>
   <si>
@@ -244,7 +247,7 @@
     <t>f</t>
   </si>
   <si>
-    <t>YYWNWl</t>
+    <t>l</t>
   </si>
   <si>
     <t>AAAA2A1</t>
@@ -725,7 +728,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -736,22 +739,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -759,22 +762,22 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -782,22 +785,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -805,22 +808,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -828,22 +831,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -851,22 +854,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -874,22 +877,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -897,22 +900,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -920,22 +923,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -943,22 +946,22 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -966,22 +969,22 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -989,22 +992,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1012,22 +1015,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1035,22 +1038,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1058,22 +1061,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1081,22 +1084,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1104,22 +1107,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1127,22 +1130,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1150,22 +1153,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G19" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1173,22 +1176,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1196,22 +1199,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
         <v>53</v>
       </c>
-      <c r="E21" t="s">
-        <v>50</v>
-      </c>
-      <c r="F21" t="s">
-        <v>52</v>
-      </c>
       <c r="G21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1219,22 +1222,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1242,22 +1245,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1265,22 +1268,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1288,22 +1291,22 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G25" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1311,22 +1314,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G26" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1334,22 +1337,22 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1357,22 +1360,22 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G28" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1380,22 +1383,22 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G29" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1403,22 +1406,22 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1426,22 +1429,22 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
+        <v>55</v>
+      </c>
+      <c r="E31" t="s">
         <v>54</v>
       </c>
-      <c r="E31" t="s">
-        <v>53</v>
-      </c>
       <c r="F31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1449,22 +1452,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1472,22 +1475,22 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F33" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1495,22 +1498,22 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" t="s">
         <v>54</v>
       </c>
-      <c r="F34" t="s">
-        <v>53</v>
-      </c>
       <c r="G34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1518,22 +1521,22 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E35" t="s">
         <v>53</v>
       </c>
       <c r="F35" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G35" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -1541,22 +1544,22 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
         <v>53</v>
       </c>
       <c r="G36" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -1564,22 +1567,22 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -1587,22 +1590,22 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E38" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" t="s">
         <v>56</v>
       </c>
-      <c r="F38" t="s">
-        <v>59</v>
-      </c>
       <c r="G38" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1610,22 +1613,22 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E39" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F39" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G39" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1633,22 +1636,22 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G40" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1656,22 +1659,22 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F41" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G41" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1679,22 +1682,22 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E42" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F42" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G42" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1702,22 +1705,22 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E43" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F43" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G43" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1725,22 +1728,22 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D44" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G44" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -1748,22 +1751,22 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E45" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F45" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G45" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1771,22 +1774,45 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" t="s">
+        <v>53</v>
+      </c>
+      <c r="E46" t="s">
+        <v>54</v>
+      </c>
+      <c r="F46" t="s">
+        <v>60</v>
+      </c>
+      <c r="G46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C46" t="s">
-        <v>46</v>
-      </c>
-      <c r="D46" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" t="s">
-        <v>52</v>
-      </c>
-      <c r="F46" t="s">
+      <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" t="s">
         <v>53</v>
       </c>
-      <c r="G46" t="s">
-        <v>65</v>
+      <c r="F47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1807,7 +1833,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1818,7 +1844,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1829,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1840,7 +1866,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1851,7 +1877,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1862,7 +1888,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1873,7 +1899,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1884,7 +1910,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1895,7 +1921,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1906,7 +1932,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1917,7 +1943,7 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -1928,7 +1954,7 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -1939,7 +1965,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -1950,7 +1976,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1961,7 +1987,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1972,7 +1998,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -1983,7 +2009,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1994,7 +2020,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -2005,7 +2031,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2016,7 +2042,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -2027,7 +2053,7 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2038,7 +2064,7 @@
         <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2049,7 +2075,7 @@
         <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2060,7 +2086,7 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2071,7 +2097,7 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2082,7 +2108,7 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2093,7 +2119,7 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2104,7 +2130,7 @@
         <v>17</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2115,7 +2141,7 @@
         <v>17</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2126,7 +2152,7 @@
         <v>18</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2137,7 +2163,7 @@
         <v>18</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2148,7 +2174,7 @@
         <v>19</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2159,7 +2185,7 @@
         <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -2170,7 +2196,7 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2181,7 +2207,7 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -2192,7 +2218,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -2203,7 +2229,7 @@
         <v>21</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -2214,7 +2240,7 @@
         <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2225,7 +2251,7 @@
         <v>22</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2236,7 +2262,7 @@
         <v>23</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -2247,7 +2273,7 @@
         <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C41">
         <v>1</v>
@@ -2258,7 +2284,7 @@
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2269,7 +2295,7 @@
         <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2280,7 +2306,7 @@
         <v>25</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -2291,7 +2317,7 @@
         <v>25</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2302,7 +2328,7 @@
         <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -2313,7 +2339,7 @@
         <v>26</v>
       </c>
       <c r="B47" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -2324,7 +2350,7 @@
         <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -2335,7 +2361,7 @@
         <v>27</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -2346,7 +2372,7 @@
         <v>28</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2357,7 +2383,7 @@
         <v>28</v>
       </c>
       <c r="B51" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -2368,7 +2394,7 @@
         <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -2379,7 +2405,7 @@
         <v>29</v>
       </c>
       <c r="B53" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -2390,7 +2416,7 @@
         <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -2401,7 +2427,7 @@
         <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -2412,7 +2438,7 @@
         <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -2423,7 +2449,7 @@
         <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -2434,7 +2460,7 @@
         <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -2445,7 +2471,7 @@
         <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -2456,7 +2482,7 @@
         <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -2467,7 +2493,7 @@
         <v>33</v>
       </c>
       <c r="B61" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C61">
         <v>1</v>
@@ -2475,10 +2501,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -2486,10 +2512,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B63" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C63">
         <v>1</v>
@@ -2497,10 +2523,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -2508,10 +2534,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C65">
         <v>1</v>
@@ -2519,10 +2545,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -2530,10 +2556,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C67">
         <v>1</v>
@@ -2541,10 +2567,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -2552,10 +2578,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -2563,10 +2589,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -2574,10 +2600,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -2585,10 +2611,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -2596,10 +2622,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B73" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -2607,10 +2633,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -2618,10 +2644,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C75">
         <v>1</v>
@@ -2629,10 +2655,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -2640,10 +2666,10 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2651,10 +2677,10 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -2662,10 +2688,10 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C79">
         <v>1</v>
@@ -2673,10 +2699,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B80" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -2684,10 +2710,10 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B81" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -2695,10 +2721,10 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B82" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -2706,10 +2732,10 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -2717,10 +2743,10 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -2728,10 +2754,10 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B85" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -2739,10 +2765,10 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B86" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -2750,10 +2776,10 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B87" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -2777,7 +2803,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C1">
         <v>-1</v>
@@ -2788,7 +2814,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C2">
         <v>-1</v>
@@ -2799,7 +2825,7 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3">
         <v>-1</v>
@@ -2810,7 +2836,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4">
         <v>-1</v>
@@ -2821,7 +2847,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>-1</v>
@@ -2832,7 +2858,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C6">
         <v>-1</v>
@@ -2843,7 +2869,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C7">
         <v>-1</v>
@@ -2854,7 +2880,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>-1</v>
@@ -2865,7 +2891,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C9">
         <v>-1</v>
@@ -2876,7 +2902,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C10">
         <v>-1</v>
@@ -2887,7 +2913,7 @@
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C11">
         <v>-1</v>
@@ -2898,7 +2924,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C12">
         <v>-1</v>
@@ -2909,7 +2935,7 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C13">
         <v>-1</v>
@@ -2920,7 +2946,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -2931,7 +2957,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>-1</v>
@@ -2942,7 +2968,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C16">
         <v>-1</v>
@@ -2953,7 +2979,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C17">
         <v>-1</v>
@@ -2964,7 +2990,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C18">
         <v>-1</v>
@@ -2975,7 +3001,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C19">
         <v>-1</v>
@@ -2986,7 +3012,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C20">
         <v>-1</v>
@@ -2997,7 +3023,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C21">
         <v>-1</v>
@@ -3008,7 +3034,7 @@
         <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C22">
         <v>-1</v>
@@ -3019,7 +3045,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C23">
         <v>-1</v>
@@ -3030,7 +3056,7 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C24">
         <v>-1</v>
@@ -3041,7 +3067,7 @@
         <v>21</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C25">
         <v>-1</v>
@@ -3052,7 +3078,7 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C26">
         <v>-1</v>
@@ -3063,7 +3089,7 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C27">
         <v>-1</v>
@@ -3074,7 +3100,7 @@
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C28">
         <v>-1</v>
@@ -3085,7 +3111,7 @@
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C29">
         <v>-1</v>
@@ -3096,7 +3122,7 @@
         <v>23</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C30">
         <v>-1</v>
@@ -3107,7 +3133,7 @@
         <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C31">
         <v>-1</v>
@@ -3118,7 +3144,7 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C32">
         <v>-1</v>
@@ -3129,7 +3155,7 @@
         <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C33">
         <v>-1</v>
@@ -3140,7 +3166,7 @@
         <v>25</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C34">
         <v>-1</v>
@@ -3151,7 +3177,7 @@
         <v>26</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C35">
         <v>-1</v>
@@ -3162,7 +3188,7 @@
         <v>26</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C36">
         <v>-1</v>
@@ -3173,7 +3199,7 @@
         <v>27</v>
       </c>
       <c r="B37" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>-1</v>
@@ -3184,7 +3210,7 @@
         <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C38">
         <v>-1</v>
@@ -3195,7 +3221,7 @@
         <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C39">
         <v>-1</v>
@@ -3206,7 +3232,7 @@
         <v>28</v>
       </c>
       <c r="B40" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C40">
         <v>-1</v>
@@ -3217,7 +3243,7 @@
         <v>29</v>
       </c>
       <c r="B41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C41">
         <v>-1</v>
@@ -3228,7 +3254,7 @@
         <v>29</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C42">
         <v>-1</v>
@@ -3239,7 +3265,7 @@
         <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C43">
         <v>-1</v>
@@ -3250,7 +3276,7 @@
         <v>30</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C44">
         <v>-1</v>
@@ -3261,7 +3287,7 @@
         <v>31</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C45">
         <v>-1</v>
@@ -3272,7 +3298,7 @@
         <v>31</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C46">
         <v>-1</v>
@@ -3283,7 +3309,7 @@
         <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C47">
         <v>-1</v>
@@ -3294,7 +3320,7 @@
         <v>32</v>
       </c>
       <c r="B48" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C48">
         <v>-1</v>
@@ -3305,7 +3331,7 @@
         <v>33</v>
       </c>
       <c r="B49" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C49">
         <v>-1</v>
@@ -3316,7 +3342,7 @@
         <v>33</v>
       </c>
       <c r="B50" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C50">
         <v>-1</v>
@@ -3324,10 +3350,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C51">
         <v>-1</v>
@@ -3335,10 +3361,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="B52" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C52">
         <v>-1</v>
@@ -3346,10 +3372,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B53" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C53">
         <v>-1</v>
@@ -3357,10 +3383,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C54">
         <v>-1</v>
@@ -3368,10 +3394,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B55" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C55">
         <v>-1</v>
@@ -3379,10 +3405,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B56" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C56">
         <v>-1</v>
@@ -3390,10 +3416,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C57">
         <v>-1</v>
@@ -3401,10 +3427,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C58">
         <v>-1</v>
@@ -3412,10 +3438,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C59">
         <v>-1</v>
@@ -3423,10 +3449,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B60" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C60">
         <v>-1</v>
@@ -3434,10 +3460,10 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C61">
         <v>-1</v>
@@ -3445,10 +3471,10 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C62">
         <v>-1</v>
@@ -3456,10 +3482,10 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B63" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C63">
         <v>-1</v>
@@ -3467,10 +3493,10 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B64" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C64">
         <v>-1</v>
@@ -3478,10 +3504,10 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B65" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C65">
         <v>-1</v>
@@ -3489,10 +3515,10 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B66" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C66">
         <v>-1</v>
@@ -3500,10 +3526,10 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B67" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C67">
         <v>-1</v>
@@ -3511,10 +3537,10 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B68" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C68">
         <v>-1</v>
@@ -3522,10 +3548,10 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C69">
         <v>-1</v>
@@ -3533,10 +3559,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C70">
         <v>-1</v>
@@ -3544,10 +3570,10 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B71" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C71">
         <v>-1</v>
@@ -3555,10 +3581,10 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B72" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C72">
         <v>-1</v>
@@ -3566,10 +3592,10 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B73" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C73">
         <v>-1</v>
@@ -3577,10 +3603,10 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B74" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C74">
         <v>-1</v>
@@ -3588,10 +3614,10 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B75" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C75">
         <v>-1</v>
@@ -3599,10 +3625,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B76" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C76">
         <v>-1</v>
@@ -3623,822 +3649,822 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F18" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E23" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F27" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E28" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F30" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" t="s">
         <v>54</v>
       </c>
-      <c r="E32" t="s">
-        <v>53</v>
-      </c>
       <c r="F32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" t="s">
         <v>53</v>
-      </c>
-      <c r="F33" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F36" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F37" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D38" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" t="s">
         <v>53</v>
-      </c>
-      <c r="E38" t="s">
-        <v>50</v>
-      </c>
-      <c r="F38" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" t="s">
         <v>54</v>
-      </c>
-      <c r="F39" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E40" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D41" t="s">
+        <v>54</v>
+      </c>
+      <c r="E41" t="s">
         <v>53</v>
       </c>
-      <c r="E41" t="s">
-        <v>52</v>
-      </c>
       <c r="F41" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>